<commit_message>
ALL module api's commited By 'Lakshmi'
</commit_message>
<xml_diff>
--- a/Ecommerce_Data_Contract.xlsx
+++ b/Ecommerce_Data_Contract.xlsx
@@ -4,12 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Database" sheetId="1" r:id="rId1"/>
     <sheet name="Endpoint Definition" sheetId="3" r:id="rId2"/>
-    <sheet name="UI Definition" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="61">
   <si>
     <t>Sl. No.</t>
   </si>
@@ -86,73 +85,10 @@
     <t>GET</t>
   </si>
   <si>
-    <t>Summary</t>
-  </si>
-  <si>
-    <t>User Interface Definition</t>
-  </si>
-  <si>
-    <t>UI Screens</t>
-  </si>
-  <si>
-    <t>Screen Description</t>
-  </si>
-  <si>
-    <t>API URL</t>
-  </si>
-  <si>
-    <t>Operation Type</t>
-  </si>
-  <si>
-    <t>Response</t>
-  </si>
-  <si>
-    <t>Screen 1</t>
-  </si>
-  <si>
-    <t>Screen 2</t>
-  </si>
-  <si>
-    <t>Screen 3</t>
-  </si>
-  <si>
-    <t>Screen 4</t>
-  </si>
-  <si>
-    <t>Screen 5</t>
-  </si>
-  <si>
-    <t>Screen 6</t>
-  </si>
-  <si>
-    <t>Screen 10</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
     <t>varchar</t>
-  </si>
-  <si>
-    <t>Account  Creation</t>
-  </si>
-  <si>
-    <t>/api/createAccount</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{
-firstName:String,
-lastName:String,
-address:String,
-age:Int
-purpose:String,
-email:String,
-city:String,
-phNum:Long,
-gender:String,
-accountType:String
-}
-</t>
   </si>
   <si>
     <t>{
@@ -161,15 +97,9 @@
 }</t>
   </si>
   <si>
-    <t>Admin Login</t>
-  </si>
-  <si>
     <t>{
 adminId: Long
 }</t>
-  </si>
-  <si>
-    <t>User Login</t>
   </si>
   <si>
     <t>/api/adminLogin</t>
@@ -203,15 +133,6 @@
   </si>
   <si>
     <t>/api/summary/{userId}</t>
-  </si>
-  <si>
-    <t>Home  Page</t>
-  </si>
-  <si>
-    <t>Admin Approval</t>
-  </si>
-  <si>
-    <t>/api/approval/{userID}</t>
   </si>
   <si>
     <t xml:space="preserve">{userId:Long,
@@ -229,9 +150,6 @@
 </t>
   </si>
   <si>
-    <t>Account Creation</t>
-  </si>
-  <si>
     <t>/api/approval/{userId}</t>
   </si>
   <si>
@@ -284,6 +202,45 @@
   </si>
   <si>
     <t>role</t>
+  </si>
+  <si>
+    <t>User Registration</t>
+  </si>
+  <si>
+    <t>updateUser</t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Add Category</t>
+  </si>
+  <si>
+    <t>Add Product</t>
+  </si>
+  <si>
+    <t>All Products</t>
+  </si>
+  <si>
+    <t>All Products By Category</t>
+  </si>
+  <si>
+    <t>Product Details</t>
+  </si>
+  <si>
+    <t>All Users</t>
+  </si>
+  <si>
+    <t>/api/addUser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+userId:Long,
+}
+</t>
   </si>
 </sst>
 </file>
@@ -369,7 +326,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -380,10 +337,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -401,9 +354,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -753,8 +703,8 @@
   </sheetPr>
   <dimension ref="A2:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -764,22 +714,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="13"/>
+      <c r="C2" s="11"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="11" t="s">
+      <c r="B4" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="9" t="s">
         <v>3</v>
       </c>
     </row>
@@ -802,7 +752,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>7</v>
@@ -814,7 +764,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>7</v>
@@ -838,7 +788,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>7</v>
@@ -856,7 +806,7 @@
         <v>0</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>2</v>
@@ -870,7 +820,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>5</v>
@@ -884,13 +834,13 @@
         <v>2</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -898,13 +848,13 @@
         <v>3</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -912,10 +862,10 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -924,7 +874,7 @@
         <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>5</v>
@@ -936,10 +886,10 @@
         <v>6</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -948,10 +898,10 @@
         <v>7</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="D19" s="1"/>
     </row>
@@ -960,7 +910,7 @@
         <v>8</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>5</v>
@@ -978,7 +928,7 @@
         <v>0</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>2</v>
@@ -992,7 +942,7 @@
         <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>5</v>
@@ -1006,13 +956,13 @@
         <v>2</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1020,10 +970,10 @@
         <v>3</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="D25" s="1"/>
     </row>
@@ -1109,8 +1059,8 @@
   </sheetPr>
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1124,212 +1074,228 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="14"/>
+      <c r="E1" s="12"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="11" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="4" customFormat="1" ht="165.75">
-      <c r="A3" s="8">
+    <row r="3" spans="1:8" s="4" customFormat="1" ht="51">
+      <c r="A3" s="6">
         <v>1</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="8" t="s">
+      <c r="B3" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
+      <c r="D3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
     </row>
     <row r="4" spans="1:8" s="4" customFormat="1" ht="165.75">
-      <c r="A4" s="8">
+      <c r="A4" s="6">
         <v>2</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="8" t="s">
+      <c r="B4" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="1:8" s="4" customFormat="1" ht="76.5">
+      <c r="A5" s="6">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+    </row>
+    <row r="6" spans="1:8" s="4" customFormat="1" ht="76.5">
+      <c r="A6" s="6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-    </row>
-    <row r="5" spans="1:8" s="4" customFormat="1" ht="76.5">
-      <c r="A5" s="8">
-        <v>3</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="8" t="s">
+      <c r="D6" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:8" ht="165.75">
+      <c r="A7" s="6">
+        <v>5</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-    </row>
-    <row r="6" spans="1:8" s="4" customFormat="1" ht="76.5">
-      <c r="A6" s="8">
-        <v>4</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-    </row>
-    <row r="7" spans="1:8" ht="165.75">
-      <c r="A7" s="8">
-        <v>5</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="9" t="s">
-        <v>52</v>
+      <c r="D7" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="7" t="s">
+        <v>30</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="8">
+      <c r="A8" s="6">
         <v>6</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="9"/>
+      <c r="B8" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="7"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="8">
+      <c r="A9" s="6">
         <v>7</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="9"/>
+      <c r="B9" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="7"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="8">
+      <c r="A10" s="6">
         <v>8</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="9"/>
+      <c r="B10" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="7"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="8">
+      <c r="A11" s="6">
         <v>9</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="9"/>
+      <c r="B11" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="7"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="8">
+      <c r="A12" s="6">
         <v>10</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="9"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="7"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="8">
+      <c r="A13" s="6">
         <v>11</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="9"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="7"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
@@ -1342,325 +1308,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr codeName="Sheet2">
-    <tabColor theme="5" tint="0.39997558519241921"/>
-  </sheetPr>
-  <dimension ref="A1:G23"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
-  <cols>
-    <col min="2" max="2" width="20.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.75" customWidth="1"/>
-    <col min="4" max="4" width="35.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="16.25" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="D1" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="15"/>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="13"/>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="1">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="1">
-        <v>2</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="1">
-        <v>3</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="1">
-        <v>4</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="1">
-        <v>5</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="1">
-        <v>6</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="1">
-        <v>7</v>
-      </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="1">
-        <v>8</v>
-      </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="1">
-        <v>9</v>
-      </c>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="1">
-        <v>10</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F4:G4"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>